<commit_message>
Add running order stats
</commit_message>
<xml_diff>
--- a/EMSC Stats Test 6 - 14.xlsx
+++ b/EMSC Stats Test 6 - 14.xlsx
@@ -408,11 +408,11 @@
     <col min="3" max="3" customWidth="1" width="23"/>
     <col min="4" max="4" customWidth="1" width="45"/>
     <col min="5" max="5" customWidth="1" width="35"/>
-    <col min="6" max="6" customWidth="1" width="3"/>
+    <col min="6" max="6" customWidth="1" width="5"/>
     <col min="7" max="7" customWidth="1" width="12"/>
-    <col min="8" max="8" customWidth="1" width="12"/>
+    <col min="8" max="8" customWidth="1" width="13"/>
     <col min="9" max="9" customWidth="1" width="13"/>
-    <col min="10" max="10" customWidth="1" width="11"/>
+    <col min="10" max="10" customWidth="1" width="12"/>
     <col min="11" max="11" customWidth="1" width="28"/>
     <col min="12" max="12" customWidth="1" width="34"/>
     <col min="13" max="13" customWidth="1" width="11"/>
@@ -445,22 +445,22 @@
         <v>Song</v>
       </c>
       <c r="F1" t="str">
-        <v>Sf</v>
+        <v xml:space="preserve"> S F</v>
       </c>
       <c r="G1" t="str">
         <v>Place Final</v>
       </c>
       <c r="H1" t="str">
-        <v>Score Final</v>
+        <v>Points Final</v>
       </c>
       <c r="I1" t="str">
         <v>Place Semi</v>
       </c>
       <c r="J1" t="str">
-        <v>Score Semi</v>
+        <v>Points Semi</v>
       </c>
       <c r="K1" t="str">
-        <v>Hod</v>
+        <v xml:space="preserve"> H O D</v>
       </c>
       <c r="L1" t="str">
         <v>Hod Short Name</v>
@@ -1701,7 +1701,7 @@
         <v>66</v>
       </c>
       <c r="K20" t="str">
-        <v>Christoph Andrianos</v>
+        <v>Richard Cox</v>
       </c>
       <c r="L20" t="str">
         <v>Richie C</v>
@@ -2091,7 +2091,7 @@
         <v>73</v>
       </c>
       <c r="K26" t="str">
-        <v>Joseph Cruz</v>
+        <v>José Mora</v>
       </c>
       <c r="L26" t="str">
         <v>Jose</v>
@@ -4431,7 +4431,7 @@
         <v>98</v>
       </c>
       <c r="K62" t="str">
-        <v>Christoph Andrianos</v>
+        <v>Richard Cox</v>
       </c>
       <c r="L62" t="str">
         <v>Richie C</v>
@@ -4626,7 +4626,7 @@
         <v>60</v>
       </c>
       <c r="K65" t="str">
-        <v>Joseph Cruz</v>
+        <v>José Mora</v>
       </c>
       <c r="L65" t="str">
         <v>Jose</v>
@@ -6836,7 +6836,7 @@
         <v>47</v>
       </c>
       <c r="K99" t="str">
-        <v>Christoph Andrianos</v>
+        <v>Richard Cox</v>
       </c>
       <c r="L99" t="str">
         <v>Richie C</v>
@@ -8656,7 +8656,7 @@
         <v>54</v>
       </c>
       <c r="K127" t="str">
-        <v>Christoph Andrianos</v>
+        <v>Richard Cox</v>
       </c>
       <c r="L127" t="str">
         <v>Richie C</v>

</xml_diff>